<commit_message>
[박청아] Add - [Item] FurnitureUnit에 SlotDatas 추가 / Fix - [Item] StorageType과 ZoneType 통합 / 코드 정리
</commit_message>
<xml_diff>
--- a/Content/TableData/ItemData.xlsx
+++ b/Content/TableData/ItemData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capark2690\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426D702E-554C-4324-A08E-83C1D835A8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCF3ADB-E974-4D71-B137-A94391AE773E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24660" yWindow="3495" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
   <si>
     <t>RowName</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>ItemName</t>
-  </si>
-  <si>
-    <t>StorageType</t>
   </si>
   <si>
     <t>TemperatureType</t>
@@ -514,22 +511,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:P17"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="13" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,111 +570,102 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>100</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>100</v>
-      </c>
-      <c r="H2" s="1">
-        <v>10000</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>100</v>
+      </c>
+      <c r="G3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>100</v>
-      </c>
-      <c r="H3" s="1">
-        <v>10000</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -686,19 +674,19 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G4" s="1">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="H4" s="1">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1">
         <v>0</v>
@@ -706,26 +694,23 @@
       <c r="J4" s="1">
         <v>0</v>
       </c>
-      <c r="K4" s="1">
-        <v>0</v>
+      <c r="K4" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -734,48 +719,45 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H5" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J5" s="1">
-        <v>100</v>
-      </c>
-      <c r="K5" s="1">
-        <v>10000</v>
+        <v>10000</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N5" s="1">
+        <v>5006</v>
       </c>
       <c r="O5" s="1">
-        <v>5006</v>
-      </c>
-      <c r="P5" s="1">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -784,48 +766,45 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H6" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J6" s="1">
-        <v>100</v>
-      </c>
-      <c r="K6" s="1">
-        <v>10000</v>
+        <v>10000</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N6" s="1">
+        <v>5004</v>
       </c>
       <c r="O6" s="1">
-        <v>5004</v>
-      </c>
-      <c r="P6" s="1">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -834,48 +813,45 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
       <c r="G7" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H7" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J7" s="1">
-        <v>100</v>
-      </c>
-      <c r="K7" s="1">
-        <v>10000</v>
+        <v>10000</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N7" s="1">
+        <v>5005</v>
       </c>
       <c r="O7" s="1">
-        <v>5005</v>
-      </c>
-      <c r="P7" s="1">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -884,48 +860,45 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J8" s="1">
-        <v>100</v>
-      </c>
-      <c r="K8" s="1">
-        <v>10000</v>
+        <v>10000</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N8" s="1">
+        <v>5008</v>
       </c>
       <c r="O8" s="1">
-        <v>5008</v>
-      </c>
-      <c r="P8" s="1">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -934,48 +907,45 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H9" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="J9" s="1">
-        <v>100</v>
-      </c>
-      <c r="K9" s="1">
-        <v>10000</v>
+        <v>10000</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N9" s="1">
+        <v>5009</v>
       </c>
       <c r="O9" s="1">
-        <v>5009</v>
-      </c>
-      <c r="P9" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -984,48 +954,45 @@
         <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H10" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I10" s="1">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="J10" s="1">
-        <v>100</v>
-      </c>
-      <c r="K10" s="1">
-        <v>10000</v>
+        <v>10000</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N10" s="1">
+        <v>5007</v>
       </c>
       <c r="O10" s="1">
-        <v>5007</v>
-      </c>
-      <c r="P10" s="1">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -1034,48 +1001,45 @@
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H11" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I11" s="1">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="J11" s="1">
-        <v>100</v>
-      </c>
-      <c r="K11" s="1">
-        <v>10000</v>
+        <v>10000</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N11" s="1">
+        <v>5001</v>
       </c>
       <c r="O11" s="1">
-        <v>5001</v>
-      </c>
-      <c r="P11" s="1">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -1084,48 +1048,45 @@
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H12" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I12" s="1">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="J12" s="1">
-        <v>100</v>
-      </c>
-      <c r="K12" s="1">
-        <v>10000</v>
+        <v>10000</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N12" s="1">
+        <v>5002</v>
       </c>
       <c r="O12" s="1">
-        <v>5002</v>
-      </c>
-      <c r="P12" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -1134,48 +1095,45 @@
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H13" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J13" s="1">
-        <v>100</v>
-      </c>
-      <c r="K13" s="1">
-        <v>10000</v>
+        <v>10000</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N13" s="1">
+        <v>5010</v>
       </c>
       <c r="O13" s="1">
-        <v>5010</v>
-      </c>
-      <c r="P13" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
@@ -1184,48 +1142,45 @@
         <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H14" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J14" s="1">
-        <v>100</v>
-      </c>
-      <c r="K14" s="1">
-        <v>10000</v>
+        <v>10000</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N14" s="1">
+        <v>5011</v>
       </c>
       <c r="O14" s="1">
-        <v>5011</v>
-      </c>
-      <c r="P14" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
@@ -1234,48 +1189,45 @@
         <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H15" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J15" s="1">
-        <v>100</v>
-      </c>
-      <c r="K15" s="1">
-        <v>10000</v>
+        <v>10000</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N15" s="1">
+        <v>5012</v>
       </c>
       <c r="O15" s="1">
-        <v>5012</v>
-      </c>
-      <c r="P15" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
@@ -1284,50 +1236,47 @@
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F16" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G16" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H16" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I16" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J16" s="1">
-        <v>100</v>
-      </c>
-      <c r="K16" s="1">
-        <v>10000</v>
+        <v>10000</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N16" s="1">
+        <v>5003</v>
       </c>
       <c r="O16" s="1">
-        <v>5003</v>
-      </c>
-      <c r="P16" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="P17" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="O17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
[박청아] Add - [Item] ItemPath 파일 설정
</commit_message>
<xml_diff>
--- a/Content/TableData/ItemData.xlsx
+++ b/Content/TableData/ItemData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capark2690\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCF3ADB-E974-4D71-B137-A94391AE773E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC4DE94-AEFA-49D3-9560-390F14324470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>RowName</t>
   </si>
@@ -66,15 +66,6 @@
     <t>PriceMax</t>
   </si>
   <si>
-    <t>StuffStaticMesh</t>
-  </si>
-  <si>
-    <t>StuffBundleStaticMesh</t>
-  </si>
-  <si>
-    <t>StuffBoxStaticMesh</t>
-  </si>
-  <si>
     <t>PathFile</t>
   </si>
   <si>
@@ -129,7 +120,12 @@
     <t>ImagePath</t>
   </si>
   <si>
-    <t>/Script/Engine.StaticMesh'/Game/3D/StaticMesh/SM_WH_BOX.SM_WH_BOX'</t>
+    <t>SlotPath100x100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemMeshPathBoxMeshPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -514,16 +510,13 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="12.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -561,21 +554,19 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="M1" s="1"/>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -584,7 +575,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -604,23 +595,25 @@
       <c r="J2" s="1">
         <v>0</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>31</v>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
       </c>
       <c r="N2" s="1">
         <v>0</v>
       </c>
-      <c r="O2" s="1"/>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -629,7 +622,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -649,23 +642,25 @@
       <c r="J3" s="1">
         <v>0</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>31</v>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
       </c>
       <c r="N3" s="1">
         <v>0</v>
       </c>
-      <c r="O3" s="1"/>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -674,7 +669,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -694,23 +689,25 @@
       <c r="J4" s="1">
         <v>0</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>31</v>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
       </c>
       <c r="N4" s="1">
         <v>0</v>
       </c>
-      <c r="O4" s="1"/>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -719,7 +716,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -739,17 +736,17 @@
       <c r="J5" s="1">
         <v>10000</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>31</v>
+      <c r="K5" s="1">
+        <v>8001</v>
+      </c>
+      <c r="L5" s="1">
+        <v>5006</v>
+      </c>
+      <c r="M5" s="1">
+        <v>6001</v>
       </c>
       <c r="N5" s="1">
-        <v>5006</v>
+        <v>7001</v>
       </c>
       <c r="O5" s="1">
         <v>101</v>
@@ -757,7 +754,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -766,7 +763,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -786,17 +783,17 @@
       <c r="J6" s="1">
         <v>10000</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>31</v>
+      <c r="K6" s="1">
+        <v>8001</v>
+      </c>
+      <c r="L6" s="1">
+        <v>5004</v>
+      </c>
+      <c r="M6" s="1">
+        <v>6001</v>
       </c>
       <c r="N6" s="1">
-        <v>5004</v>
+        <v>7001</v>
       </c>
       <c r="O6" s="1">
         <v>102</v>
@@ -804,7 +801,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -813,7 +810,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -833,17 +830,17 @@
       <c r="J7" s="1">
         <v>10000</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>31</v>
+      <c r="K7" s="1">
+        <v>8001</v>
+      </c>
+      <c r="L7" s="1">
+        <v>5005</v>
+      </c>
+      <c r="M7" s="1">
+        <v>6001</v>
       </c>
       <c r="N7" s="1">
-        <v>5005</v>
+        <v>7001</v>
       </c>
       <c r="O7" s="1">
         <v>103</v>
@@ -851,7 +848,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -860,7 +857,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -880,17 +877,17 @@
       <c r="J8" s="1">
         <v>10000</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>31</v>
+      <c r="K8" s="1">
+        <v>8001</v>
+      </c>
+      <c r="L8" s="1">
+        <v>5008</v>
+      </c>
+      <c r="M8" s="1">
+        <v>6001</v>
       </c>
       <c r="N8" s="1">
-        <v>5008</v>
+        <v>7001</v>
       </c>
       <c r="O8" s="1">
         <v>104</v>
@@ -898,7 +895,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -907,7 +904,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
@@ -927,17 +924,17 @@
       <c r="J9" s="1">
         <v>10000</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>31</v>
+      <c r="K9" s="1">
+        <v>8001</v>
+      </c>
+      <c r="L9" s="1">
+        <v>5009</v>
+      </c>
+      <c r="M9" s="1">
+        <v>6001</v>
       </c>
       <c r="N9" s="1">
-        <v>5009</v>
+        <v>7001</v>
       </c>
       <c r="O9" s="1">
         <v>105</v>
@@ -945,7 +942,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -954,7 +951,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -974,17 +971,17 @@
       <c r="J10" s="1">
         <v>10000</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>31</v>
+      <c r="K10" s="1">
+        <v>8001</v>
+      </c>
+      <c r="L10" s="1">
+        <v>5007</v>
+      </c>
+      <c r="M10" s="1">
+        <v>6001</v>
       </c>
       <c r="N10" s="1">
-        <v>5007</v>
+        <v>7001</v>
       </c>
       <c r="O10" s="1">
         <v>106</v>
@@ -992,7 +989,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -1001,7 +998,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E11" s="1">
         <v>3</v>
@@ -1021,17 +1018,17 @@
       <c r="J11" s="1">
         <v>10000</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>31</v>
+      <c r="K11" s="1">
+        <v>8001</v>
+      </c>
+      <c r="L11" s="1">
+        <v>5001</v>
+      </c>
+      <c r="M11" s="1">
+        <v>6001</v>
       </c>
       <c r="N11" s="1">
-        <v>5001</v>
+        <v>7001</v>
       </c>
       <c r="O11" s="1">
         <v>107</v>
@@ -1039,7 +1036,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -1048,7 +1045,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
@@ -1068,17 +1065,17 @@
       <c r="J12" s="1">
         <v>10000</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>31</v>
+      <c r="K12" s="1">
+        <v>8001</v>
+      </c>
+      <c r="L12" s="1">
+        <v>5002</v>
+      </c>
+      <c r="M12" s="1">
+        <v>6001</v>
       </c>
       <c r="N12" s="1">
-        <v>5002</v>
+        <v>7001</v>
       </c>
       <c r="O12" s="1">
         <v>108</v>
@@ -1086,7 +1083,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -1095,7 +1092,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
@@ -1115,17 +1112,17 @@
       <c r="J13" s="1">
         <v>10000</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>31</v>
+      <c r="K13" s="1">
+        <v>8001</v>
+      </c>
+      <c r="L13" s="1">
+        <v>5010</v>
+      </c>
+      <c r="M13" s="1">
+        <v>6001</v>
       </c>
       <c r="N13" s="1">
-        <v>5010</v>
+        <v>7001</v>
       </c>
       <c r="O13" s="1">
         <v>109</v>
@@ -1133,7 +1130,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
@@ -1142,7 +1139,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
@@ -1162,17 +1159,17 @@
       <c r="J14" s="1">
         <v>10000</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>31</v>
+      <c r="K14" s="1">
+        <v>8001</v>
+      </c>
+      <c r="L14" s="1">
+        <v>5011</v>
+      </c>
+      <c r="M14" s="1">
+        <v>6001</v>
       </c>
       <c r="N14" s="1">
-        <v>5011</v>
+        <v>7001</v>
       </c>
       <c r="O14" s="1">
         <v>110</v>
@@ -1180,7 +1177,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
@@ -1189,7 +1186,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
@@ -1209,17 +1206,17 @@
       <c r="J15" s="1">
         <v>10000</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>31</v>
+      <c r="K15" s="1">
+        <v>8001</v>
+      </c>
+      <c r="L15" s="1">
+        <v>5012</v>
+      </c>
+      <c r="M15" s="1">
+        <v>6001</v>
       </c>
       <c r="N15" s="1">
-        <v>5012</v>
+        <v>7001</v>
       </c>
       <c r="O15" s="1">
         <v>111</v>
@@ -1227,7 +1224,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
@@ -1236,7 +1233,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E16" s="1">
         <v>3</v>
@@ -1256,17 +1253,17 @@
       <c r="J16" s="1">
         <v>10000</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>31</v>
+      <c r="K16" s="1">
+        <v>8001</v>
+      </c>
+      <c r="L16" s="1">
+        <v>5003</v>
+      </c>
+      <c r="M16" s="1">
+        <v>6001</v>
       </c>
       <c r="N16" s="1">
-        <v>5003</v>
+        <v>7001</v>
       </c>
       <c r="O16" s="1">
         <v>112</v>
@@ -1274,7 +1271,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O17" s="1"/>
     </row>

</xml_diff>

<commit_message>
[박청아] Add - [Item] Slot Status Widget을 통한 아이템 이동
</commit_message>
<xml_diff>
--- a/Content/TableData/ItemData.xlsx
+++ b/Content/TableData/ItemData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capark2690\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE8F08B-8E90-4D23-837A-3D17EA19CD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013521EA-4FAC-48BA-9AF2-D4E1D6519658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
   <si>
     <t>RowName</t>
   </si>
@@ -197,6 +197,14 @@
   </si>
   <si>
     <t>MilkG</t>
+  </si>
+  <si>
+    <t>Slot100x100MaxCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoxMaxCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -578,19 +586,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="5" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,29 +615,35 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1"/>
+      <c r="N1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -646,16 +660,16 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -669,8 +683,14 @@
       <c r="M2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -687,16 +707,16 @@
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -710,8 +730,14 @@
       <c r="M3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -728,16 +754,16 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
@@ -751,8 +777,14 @@
       <c r="M4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -769,31 +801,37 @@
         <v>2</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G5" s="1">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H5" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J5" s="1">
+        <v>100</v>
+      </c>
+      <c r="K5" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L5" s="1">
         <v>8004</v>
       </c>
-      <c r="K5" s="1">
-        <v>6001</v>
-      </c>
-      <c r="L5" s="1">
-        <v>7001</v>
-      </c>
       <c r="M5" s="1">
+        <v>6001</v>
+      </c>
+      <c r="N5" s="1">
+        <v>7001</v>
+      </c>
+      <c r="O5" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -810,31 +848,37 @@
         <v>2</v>
       </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G6" s="1">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H6" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J6" s="1">
+        <v>100</v>
+      </c>
+      <c r="K6" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L6" s="1">
         <v>8005</v>
       </c>
-      <c r="K6" s="1">
-        <v>6001</v>
-      </c>
-      <c r="L6" s="1">
-        <v>7001</v>
-      </c>
       <c r="M6" s="1">
+        <v>6001</v>
+      </c>
+      <c r="N6" s="1">
+        <v>7001</v>
+      </c>
+      <c r="O6" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -851,31 +895,37 @@
         <v>2</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G7" s="1">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H7" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J7" s="1">
+        <v>100</v>
+      </c>
+      <c r="K7" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L7" s="1">
         <v>8006</v>
       </c>
-      <c r="K7" s="1">
-        <v>6001</v>
-      </c>
-      <c r="L7" s="1">
-        <v>7001</v>
-      </c>
       <c r="M7" s="1">
+        <v>6001</v>
+      </c>
+      <c r="N7" s="1">
+        <v>7001</v>
+      </c>
+      <c r="O7" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -892,31 +942,37 @@
         <v>3</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G8" s="1">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H8" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J8" s="1">
+        <v>100</v>
+      </c>
+      <c r="K8" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L8" s="1">
         <v>8007</v>
       </c>
-      <c r="K8" s="1">
-        <v>6001</v>
-      </c>
-      <c r="L8" s="1">
-        <v>7001</v>
-      </c>
       <c r="M8" s="1">
+        <v>6001</v>
+      </c>
+      <c r="N8" s="1">
+        <v>7001</v>
+      </c>
+      <c r="O8" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -933,31 +989,37 @@
         <v>3</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G9" s="1">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H9" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J9" s="1">
+        <v>100</v>
+      </c>
+      <c r="K9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L9" s="1">
         <v>8008</v>
       </c>
-      <c r="K9" s="1">
-        <v>6001</v>
-      </c>
-      <c r="L9" s="1">
-        <v>7001</v>
-      </c>
       <c r="M9" s="1">
+        <v>6001</v>
+      </c>
+      <c r="N9" s="1">
+        <v>7001</v>
+      </c>
+      <c r="O9" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -974,31 +1036,37 @@
         <v>3</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G10" s="1">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H10" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I10" s="1">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J10" s="1">
+        <v>100</v>
+      </c>
+      <c r="K10" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L10" s="1">
         <v>8009</v>
       </c>
-      <c r="K10" s="1">
-        <v>6001</v>
-      </c>
-      <c r="L10" s="1">
-        <v>7001</v>
-      </c>
       <c r="M10" s="1">
+        <v>6001</v>
+      </c>
+      <c r="N10" s="1">
+        <v>7001</v>
+      </c>
+      <c r="O10" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1015,31 +1083,37 @@
         <v>3</v>
       </c>
       <c r="F11" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G11" s="1">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H11" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J11" s="1">
+        <v>100</v>
+      </c>
+      <c r="K11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L11" s="1">
         <v>8010</v>
       </c>
-      <c r="K11" s="1">
-        <v>6001</v>
-      </c>
-      <c r="L11" s="1">
-        <v>7001</v>
-      </c>
       <c r="M11" s="1">
+        <v>6001</v>
+      </c>
+      <c r="N11" s="1">
+        <v>7001</v>
+      </c>
+      <c r="O11" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1056,31 +1130,37 @@
         <v>3</v>
       </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G12" s="1">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H12" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J12" s="1">
+        <v>100</v>
+      </c>
+      <c r="K12" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L12" s="1">
         <v>8011</v>
       </c>
-      <c r="K12" s="1">
-        <v>6001</v>
-      </c>
-      <c r="L12" s="1">
-        <v>7001</v>
-      </c>
       <c r="M12" s="1">
+        <v>6001</v>
+      </c>
+      <c r="N12" s="1">
+        <v>7001</v>
+      </c>
+      <c r="O12" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1097,31 +1177,37 @@
         <v>3</v>
       </c>
       <c r="F13" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G13" s="1">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H13" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J13" s="1">
+        <v>100</v>
+      </c>
+      <c r="K13" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L13" s="1">
         <v>8012</v>
       </c>
-      <c r="K13" s="1">
-        <v>6001</v>
-      </c>
-      <c r="L13" s="1">
-        <v>7001</v>
-      </c>
       <c r="M13" s="1">
+        <v>6001</v>
+      </c>
+      <c r="N13" s="1">
+        <v>7001</v>
+      </c>
+      <c r="O13" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1138,31 +1224,37 @@
         <v>3</v>
       </c>
       <c r="F14" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G14" s="1">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H14" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J14" s="1">
+        <v>100</v>
+      </c>
+      <c r="K14" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L14" s="1">
         <v>8013</v>
       </c>
-      <c r="K14" s="1">
-        <v>6001</v>
-      </c>
-      <c r="L14" s="1">
-        <v>7001</v>
-      </c>
       <c r="M14" s="1">
+        <v>6001</v>
+      </c>
+      <c r="N14" s="1">
+        <v>7001</v>
+      </c>
+      <c r="O14" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1179,31 +1271,37 @@
         <v>3</v>
       </c>
       <c r="F15" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G15" s="1">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H15" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J15" s="1">
+        <v>100</v>
+      </c>
+      <c r="K15" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L15" s="1">
         <v>8014</v>
       </c>
-      <c r="K15" s="1">
-        <v>6001</v>
-      </c>
-      <c r="L15" s="1">
-        <v>7001</v>
-      </c>
       <c r="M15" s="1">
+        <v>6001</v>
+      </c>
+      <c r="N15" s="1">
+        <v>7001</v>
+      </c>
+      <c r="O15" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1220,31 +1318,37 @@
         <v>3</v>
       </c>
       <c r="F16" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G16" s="1">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H16" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I16" s="1">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J16" s="1">
+        <v>100</v>
+      </c>
+      <c r="K16" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L16" s="1">
         <v>8015</v>
       </c>
-      <c r="K16" s="1">
-        <v>6001</v>
-      </c>
-      <c r="L16" s="1">
-        <v>7001</v>
-      </c>
       <c r="M16" s="1">
+        <v>6001</v>
+      </c>
+      <c r="N16" s="1">
+        <v>7001</v>
+      </c>
+      <c r="O16" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1260,32 +1364,38 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>4</v>
+      <c r="F17" s="1">
+        <v>16</v>
+      </c>
+      <c r="G17" s="1">
+        <v>100</v>
       </c>
       <c r="H17">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J17">
+        <v>100</v>
+      </c>
+      <c r="K17">
+        <v>10000</v>
+      </c>
+      <c r="L17">
         <v>8016</v>
       </c>
-      <c r="K17">
-        <v>6001</v>
-      </c>
-      <c r="L17">
-        <v>7001</v>
-      </c>
-      <c r="M17" s="1">
+      <c r="M17">
+        <v>6001</v>
+      </c>
+      <c r="N17">
+        <v>7001</v>
+      </c>
+      <c r="O17" s="1">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>17</v>
       </c>
@@ -1298,32 +1408,38 @@
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>4</v>
+      <c r="F18" s="1">
+        <v>16</v>
+      </c>
+      <c r="G18" s="1">
+        <v>100</v>
       </c>
       <c r="H18">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I18">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J18">
+        <v>100</v>
+      </c>
+      <c r="K18">
+        <v>10000</v>
+      </c>
+      <c r="L18">
         <v>8017</v>
       </c>
-      <c r="K18">
-        <v>6001</v>
-      </c>
-      <c r="L18">
-        <v>7001</v>
-      </c>
       <c r="M18">
+        <v>6001</v>
+      </c>
+      <c r="N18">
+        <v>7001</v>
+      </c>
+      <c r="O18">
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>18</v>
       </c>
@@ -1336,32 +1452,38 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>4</v>
+      <c r="F19" s="1">
+        <v>16</v>
+      </c>
+      <c r="G19" s="1">
+        <v>100</v>
       </c>
       <c r="H19">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J19">
+        <v>100</v>
+      </c>
+      <c r="K19">
+        <v>10000</v>
+      </c>
+      <c r="L19">
         <v>8018</v>
       </c>
-      <c r="K19">
-        <v>6001</v>
-      </c>
-      <c r="L19">
-        <v>7001</v>
-      </c>
       <c r="M19">
+        <v>6001</v>
+      </c>
+      <c r="N19">
+        <v>7001</v>
+      </c>
+      <c r="O19">
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>19</v>
       </c>
@@ -1374,32 +1496,38 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>4</v>
+      <c r="F20" s="1">
+        <v>16</v>
+      </c>
+      <c r="G20" s="1">
+        <v>100</v>
       </c>
       <c r="H20">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J20">
+        <v>100</v>
+      </c>
+      <c r="K20">
+        <v>10000</v>
+      </c>
+      <c r="L20">
         <v>8019</v>
       </c>
-      <c r="K20">
-        <v>6001</v>
-      </c>
-      <c r="L20">
-        <v>7001</v>
-      </c>
       <c r="M20">
+        <v>6001</v>
+      </c>
+      <c r="N20">
+        <v>7001</v>
+      </c>
+      <c r="O20">
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>20</v>
       </c>
@@ -1412,32 +1540,38 @@
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>4</v>
+      <c r="F21" s="1">
+        <v>16</v>
+      </c>
+      <c r="G21" s="1">
+        <v>100</v>
       </c>
       <c r="H21">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J21">
+        <v>100</v>
+      </c>
+      <c r="K21">
+        <v>10000</v>
+      </c>
+      <c r="L21">
         <v>8020</v>
       </c>
-      <c r="K21">
-        <v>6001</v>
-      </c>
-      <c r="L21">
-        <v>7001</v>
-      </c>
       <c r="M21">
+        <v>6001</v>
+      </c>
+      <c r="N21">
+        <v>7001</v>
+      </c>
+      <c r="O21">
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>21</v>
       </c>
@@ -1450,32 +1584,38 @@
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>4</v>
+      <c r="F22" s="1">
+        <v>16</v>
+      </c>
+      <c r="G22" s="1">
+        <v>100</v>
       </c>
       <c r="H22">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J22">
+        <v>100</v>
+      </c>
+      <c r="K22">
+        <v>10000</v>
+      </c>
+      <c r="L22">
         <v>8021</v>
       </c>
-      <c r="K22">
-        <v>6001</v>
-      </c>
-      <c r="L22">
-        <v>7001</v>
-      </c>
       <c r="M22">
+        <v>6001</v>
+      </c>
+      <c r="N22">
+        <v>7001</v>
+      </c>
+      <c r="O22">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>22</v>
       </c>
@@ -1488,32 +1628,38 @@
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>4</v>
+      <c r="F23" s="1">
+        <v>16</v>
+      </c>
+      <c r="G23" s="1">
+        <v>100</v>
       </c>
       <c r="H23">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J23">
+        <v>100</v>
+      </c>
+      <c r="K23">
+        <v>10000</v>
+      </c>
+      <c r="L23">
         <v>8022</v>
       </c>
-      <c r="K23">
-        <v>6001</v>
-      </c>
-      <c r="L23">
-        <v>7001</v>
-      </c>
       <c r="M23">
+        <v>6001</v>
+      </c>
+      <c r="N23">
+        <v>7001</v>
+      </c>
+      <c r="O23">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>23</v>
       </c>
@@ -1526,32 +1672,38 @@
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>4</v>
+      <c r="F24" s="1">
+        <v>16</v>
+      </c>
+      <c r="G24" s="1">
+        <v>100</v>
       </c>
       <c r="H24">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J24">
+        <v>100</v>
+      </c>
+      <c r="K24">
+        <v>10000</v>
+      </c>
+      <c r="L24">
         <v>8023</v>
       </c>
-      <c r="K24">
-        <v>6001</v>
-      </c>
-      <c r="L24">
-        <v>7001</v>
-      </c>
       <c r="M24">
+        <v>6001</v>
+      </c>
+      <c r="N24">
+        <v>7001</v>
+      </c>
+      <c r="O24">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>24</v>
       </c>
@@ -1564,32 +1716,38 @@
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>4</v>
+      <c r="F25" s="1">
+        <v>16</v>
+      </c>
+      <c r="G25" s="1">
+        <v>100</v>
       </c>
       <c r="H25">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J25">
+        <v>100</v>
+      </c>
+      <c r="K25">
+        <v>10000</v>
+      </c>
+      <c r="L25">
         <v>8024</v>
       </c>
-      <c r="K25">
-        <v>6001</v>
-      </c>
-      <c r="L25">
-        <v>7001</v>
-      </c>
       <c r="M25">
+        <v>6001</v>
+      </c>
+      <c r="N25">
+        <v>7001</v>
+      </c>
+      <c r="O25">
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>25</v>
       </c>
@@ -1602,32 +1760,38 @@
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>4</v>
+      <c r="F26" s="1">
+        <v>16</v>
+      </c>
+      <c r="G26" s="1">
+        <v>100</v>
       </c>
       <c r="H26">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J26">
+        <v>100</v>
+      </c>
+      <c r="K26">
+        <v>10000</v>
+      </c>
+      <c r="L26">
         <v>8025</v>
       </c>
-      <c r="K26">
-        <v>6001</v>
-      </c>
-      <c r="L26">
-        <v>7001</v>
-      </c>
       <c r="M26">
+        <v>6001</v>
+      </c>
+      <c r="N26">
+        <v>7001</v>
+      </c>
+      <c r="O26">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>26</v>
       </c>
@@ -1640,32 +1804,38 @@
       <c r="E27">
         <v>3</v>
       </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>4</v>
+      <c r="F27" s="1">
+        <v>16</v>
+      </c>
+      <c r="G27" s="1">
+        <v>100</v>
       </c>
       <c r="H27">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J27">
+        <v>100</v>
+      </c>
+      <c r="K27">
+        <v>10000</v>
+      </c>
+      <c r="L27">
         <v>8026</v>
       </c>
-      <c r="K27">
-        <v>6001</v>
-      </c>
-      <c r="L27">
-        <v>7001</v>
-      </c>
       <c r="M27">
+        <v>6001</v>
+      </c>
+      <c r="N27">
+        <v>7001</v>
+      </c>
+      <c r="O27">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>27</v>
       </c>
@@ -1678,32 +1848,38 @@
       <c r="E28">
         <v>3</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>4</v>
+      <c r="F28" s="1">
+        <v>16</v>
+      </c>
+      <c r="G28" s="1">
+        <v>100</v>
       </c>
       <c r="H28">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I28">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J28">
+        <v>100</v>
+      </c>
+      <c r="K28">
+        <v>10000</v>
+      </c>
+      <c r="L28">
         <v>8027</v>
       </c>
-      <c r="K28">
-        <v>6001</v>
-      </c>
-      <c r="L28">
-        <v>7001</v>
-      </c>
       <c r="M28">
+        <v>6001</v>
+      </c>
+      <c r="N28">
+        <v>7001</v>
+      </c>
+      <c r="O28">
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>28</v>
       </c>
@@ -1716,32 +1892,38 @@
       <c r="E29">
         <v>3</v>
       </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>4</v>
+      <c r="F29" s="1">
+        <v>16</v>
+      </c>
+      <c r="G29" s="1">
+        <v>100</v>
       </c>
       <c r="H29">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I29">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J29">
+        <v>100</v>
+      </c>
+      <c r="K29">
+        <v>10000</v>
+      </c>
+      <c r="L29">
         <v>8028</v>
       </c>
-      <c r="K29">
-        <v>6001</v>
-      </c>
-      <c r="L29">
-        <v>7001</v>
-      </c>
       <c r="M29">
+        <v>6001</v>
+      </c>
+      <c r="N29">
+        <v>7001</v>
+      </c>
+      <c r="O29">
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>29</v>
       </c>
@@ -1754,32 +1936,38 @@
       <c r="E30">
         <v>2</v>
       </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <v>4</v>
+      <c r="F30" s="1">
+        <v>16</v>
+      </c>
+      <c r="G30" s="1">
+        <v>100</v>
       </c>
       <c r="H30">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I30">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J30">
+        <v>100</v>
+      </c>
+      <c r="K30">
+        <v>10000</v>
+      </c>
+      <c r="L30">
         <v>8029</v>
       </c>
-      <c r="K30">
-        <v>6001</v>
-      </c>
-      <c r="L30">
-        <v>7001</v>
-      </c>
       <c r="M30">
+        <v>6001</v>
+      </c>
+      <c r="N30">
+        <v>7001</v>
+      </c>
+      <c r="O30">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>30</v>
       </c>
@@ -1792,32 +1980,38 @@
       <c r="E31">
         <v>2</v>
       </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31">
-        <v>4</v>
+      <c r="F31" s="1">
+        <v>16</v>
+      </c>
+      <c r="G31" s="1">
+        <v>100</v>
       </c>
       <c r="H31">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I31">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J31">
+        <v>100</v>
+      </c>
+      <c r="K31">
+        <v>10000</v>
+      </c>
+      <c r="L31">
         <v>8030</v>
       </c>
-      <c r="K31">
-        <v>6001</v>
-      </c>
-      <c r="L31">
-        <v>7001</v>
-      </c>
       <c r="M31">
+        <v>6001</v>
+      </c>
+      <c r="N31">
+        <v>7001</v>
+      </c>
+      <c r="O31">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>31</v>
       </c>
@@ -1830,32 +2024,38 @@
       <c r="E32">
         <v>2</v>
       </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <v>4</v>
+      <c r="F32" s="1">
+        <v>16</v>
+      </c>
+      <c r="G32" s="1">
+        <v>100</v>
       </c>
       <c r="H32">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I32">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J32">
+        <v>100</v>
+      </c>
+      <c r="K32">
+        <v>10000</v>
+      </c>
+      <c r="L32">
         <v>8031</v>
       </c>
-      <c r="K32">
-        <v>6001</v>
-      </c>
-      <c r="L32">
-        <v>7001</v>
-      </c>
       <c r="M32">
+        <v>6001</v>
+      </c>
+      <c r="N32">
+        <v>7001</v>
+      </c>
+      <c r="O32">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>32</v>
       </c>
@@ -1868,32 +2068,38 @@
       <c r="E33">
         <v>2</v>
       </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>4</v>
+      <c r="F33" s="1">
+        <v>16</v>
+      </c>
+      <c r="G33" s="1">
+        <v>100</v>
       </c>
       <c r="H33">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J33">
+        <v>100</v>
+      </c>
+      <c r="K33">
+        <v>10000</v>
+      </c>
+      <c r="L33">
         <v>8032</v>
       </c>
-      <c r="K33">
-        <v>6001</v>
-      </c>
-      <c r="L33">
-        <v>7001</v>
-      </c>
       <c r="M33">
+        <v>6001</v>
+      </c>
+      <c r="N33">
+        <v>7001</v>
+      </c>
+      <c r="O33">
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>33</v>
       </c>
@@ -1906,32 +2112,38 @@
       <c r="E34">
         <v>2</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34">
-        <v>4</v>
+      <c r="F34" s="1">
+        <v>16</v>
+      </c>
+      <c r="G34" s="1">
+        <v>100</v>
       </c>
       <c r="H34">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I34">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J34">
+        <v>100</v>
+      </c>
+      <c r="K34">
+        <v>10000</v>
+      </c>
+      <c r="L34">
         <v>8033</v>
       </c>
-      <c r="K34">
-        <v>6001</v>
-      </c>
-      <c r="L34">
-        <v>7001</v>
-      </c>
       <c r="M34">
+        <v>6001</v>
+      </c>
+      <c r="N34">
+        <v>7001</v>
+      </c>
+      <c r="O34">
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>34</v>
       </c>
@@ -1944,32 +2156,38 @@
       <c r="E35">
         <v>2</v>
       </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35">
-        <v>4</v>
+      <c r="F35" s="1">
+        <v>16</v>
+      </c>
+      <c r="G35" s="1">
+        <v>100</v>
       </c>
       <c r="H35">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I35">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J35">
+        <v>100</v>
+      </c>
+      <c r="K35">
+        <v>10000</v>
+      </c>
+      <c r="L35">
         <v>8034</v>
       </c>
-      <c r="K35">
-        <v>6001</v>
-      </c>
-      <c r="L35">
-        <v>7001</v>
-      </c>
       <c r="M35">
+        <v>6001</v>
+      </c>
+      <c r="N35">
+        <v>7001</v>
+      </c>
+      <c r="O35">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>35</v>
       </c>
@@ -1982,32 +2200,38 @@
       <c r="E36">
         <v>2</v>
       </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>4</v>
+      <c r="F36" s="1">
+        <v>16</v>
+      </c>
+      <c r="G36" s="1">
+        <v>100</v>
       </c>
       <c r="H36">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I36">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J36">
+        <v>100</v>
+      </c>
+      <c r="K36">
+        <v>10000</v>
+      </c>
+      <c r="L36">
         <v>8035</v>
       </c>
-      <c r="K36">
-        <v>6001</v>
-      </c>
-      <c r="L36">
-        <v>7001</v>
-      </c>
       <c r="M36">
+        <v>6001</v>
+      </c>
+      <c r="N36">
+        <v>7001</v>
+      </c>
+      <c r="O36">
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>36</v>
       </c>
@@ -2020,32 +2244,38 @@
       <c r="E37">
         <v>2</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37">
-        <v>4</v>
+      <c r="F37" s="1">
+        <v>16</v>
+      </c>
+      <c r="G37" s="1">
+        <v>100</v>
       </c>
       <c r="H37">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I37">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J37">
+        <v>100</v>
+      </c>
+      <c r="K37">
+        <v>10000</v>
+      </c>
+      <c r="L37">
         <v>8036</v>
       </c>
-      <c r="K37">
-        <v>6001</v>
-      </c>
-      <c r="L37">
-        <v>7001</v>
-      </c>
       <c r="M37">
+        <v>6001</v>
+      </c>
+      <c r="N37">
+        <v>7001</v>
+      </c>
+      <c r="O37">
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>37</v>
       </c>
@@ -2058,32 +2288,38 @@
       <c r="E38">
         <v>2</v>
       </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="G38">
-        <v>4</v>
+      <c r="F38" s="1">
+        <v>16</v>
+      </c>
+      <c r="G38" s="1">
+        <v>100</v>
       </c>
       <c r="H38">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I38">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J38">
+        <v>100</v>
+      </c>
+      <c r="K38">
+        <v>10000</v>
+      </c>
+      <c r="L38">
         <v>8037</v>
       </c>
-      <c r="K38">
-        <v>6001</v>
-      </c>
-      <c r="L38">
-        <v>7001</v>
-      </c>
       <c r="M38">
+        <v>6001</v>
+      </c>
+      <c r="N38">
+        <v>7001</v>
+      </c>
+      <c r="O38">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>38</v>
       </c>
@@ -2096,32 +2332,38 @@
       <c r="E39">
         <v>2</v>
       </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39">
-        <v>4</v>
+      <c r="F39" s="1">
+        <v>16</v>
+      </c>
+      <c r="G39" s="1">
+        <v>100</v>
       </c>
       <c r="H39">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I39">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J39">
+        <v>100</v>
+      </c>
+      <c r="K39">
+        <v>10000</v>
+      </c>
+      <c r="L39">
         <v>8038</v>
       </c>
-      <c r="K39">
-        <v>6001</v>
-      </c>
-      <c r="L39">
-        <v>7001</v>
-      </c>
       <c r="M39">
+        <v>6001</v>
+      </c>
+      <c r="N39">
+        <v>7001</v>
+      </c>
+      <c r="O39">
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>39</v>
       </c>
@@ -2134,32 +2376,38 @@
       <c r="E40">
         <v>2</v>
       </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40">
-        <v>4</v>
+      <c r="F40" s="1">
+        <v>16</v>
+      </c>
+      <c r="G40" s="1">
+        <v>100</v>
       </c>
       <c r="H40">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I40">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J40">
+        <v>100</v>
+      </c>
+      <c r="K40">
+        <v>10000</v>
+      </c>
+      <c r="L40">
         <v>8039</v>
       </c>
-      <c r="K40">
-        <v>6001</v>
-      </c>
-      <c r="L40">
-        <v>7001</v>
-      </c>
       <c r="M40">
+        <v>6001</v>
+      </c>
+      <c r="N40">
+        <v>7001</v>
+      </c>
+      <c r="O40">
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>40</v>
       </c>
@@ -2172,32 +2420,38 @@
       <c r="E41">
         <v>2</v>
       </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
-      <c r="G41">
-        <v>4</v>
+      <c r="F41" s="1">
+        <v>16</v>
+      </c>
+      <c r="G41" s="1">
+        <v>100</v>
       </c>
       <c r="H41">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J41">
+        <v>100</v>
+      </c>
+      <c r="K41">
+        <v>10000</v>
+      </c>
+      <c r="L41">
         <v>8040</v>
       </c>
-      <c r="K41">
-        <v>6001</v>
-      </c>
-      <c r="L41">
-        <v>7001</v>
-      </c>
       <c r="M41">
+        <v>6001</v>
+      </c>
+      <c r="N41">
+        <v>7001</v>
+      </c>
+      <c r="O41">
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>41</v>
       </c>
@@ -2210,28 +2464,34 @@
       <c r="E42">
         <v>2</v>
       </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42">
-        <v>4</v>
+      <c r="F42" s="1">
+        <v>16</v>
+      </c>
+      <c r="G42" s="1">
+        <v>100</v>
       </c>
       <c r="H42">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="J42">
+        <v>100</v>
+      </c>
+      <c r="K42">
+        <v>10000</v>
+      </c>
+      <c r="L42">
         <v>8041</v>
       </c>
-      <c r="K42">
-        <v>6001</v>
-      </c>
-      <c r="L42">
-        <v>7001</v>
-      </c>
       <c r="M42">
+        <v>6001</v>
+      </c>
+      <c r="N42">
+        <v>7001</v>
+      </c>
+      <c r="O42">
         <v>106</v>
       </c>
     </row>

</xml_diff>